<commit_message>
Medidos los 2 diodos
</commit_message>
<xml_diff>
--- a/1erParte/a.Diodo Rectificador/Mediciones_1N4007.xlsx
+++ b/1erParte/a.Diodo Rectificador/Mediciones_1N4007.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68952A31-A591-41B7-81CF-9A32944742B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2D6709-AACE-414A-87FC-6902B9F7CBA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -408,7 +408,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,7 +454,9 @@
       <c r="B3" s="4">
         <v>0</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
       <c r="D3" s="4">
         <f>(B3-C3)/1200</f>
         <v>0</v>
@@ -472,12 +474,14 @@
     <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="C4" s="4"/>
+        <v>0.106</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.106</v>
+      </c>
       <c r="D4" s="4">
         <f t="shared" ref="D4:D20" si="0">(B4-C4)/1200</f>
-        <v>8.3333333333333344E-5</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -492,12 +496,14 @@
     <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="C5" s="4"/>
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.20499999999999999</v>
+      </c>
       <c r="D5" s="4">
         <f t="shared" si="0"/>
-        <v>1.6666666666666669E-4</v>
+        <v>0</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -512,12 +518,14 @@
     <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="C6" s="4"/>
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.30399999999999999</v>
+      </c>
       <c r="D6" s="4">
         <f t="shared" si="0"/>
-        <v>2.5000000000000001E-4</v>
+        <v>8.3333333333333407E-7</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -532,12 +540,14 @@
     <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="4">
-        <v>0.35</v>
-      </c>
-      <c r="C7" s="4"/>
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.35099999999999998</v>
+      </c>
       <c r="D7" s="4">
         <f t="shared" si="0"/>
-        <v>2.9166666666666664E-4</v>
+        <v>3.3333333333333363E-6</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -552,12 +562,14 @@
     <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="C8" s="4"/>
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.39300000000000002</v>
+      </c>
       <c r="D8" s="4">
         <f t="shared" si="0"/>
-        <v>3.3333333333333338E-4</v>
+        <v>9.1666666666666749E-6</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -572,12 +584,14 @@
     <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="4">
-        <v>0.45</v>
-      </c>
-      <c r="C9" s="4"/>
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.42699999999999999</v>
+      </c>
       <c r="D9" s="4">
         <f t="shared" si="0"/>
-        <v>3.7500000000000001E-4</v>
+        <v>2.3333333333333353E-5</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -592,12 +606,14 @@
     <row r="10" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C10" s="4"/>
+        <v>0.504</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.45100000000000001</v>
+      </c>
       <c r="D10" s="4">
         <f t="shared" si="0"/>
-        <v>4.1666666666666669E-4</v>
+        <v>4.4166666666666658E-5</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -612,12 +628,14 @@
     <row r="11" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="4">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="C11" s="4"/>
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.46899999999999997</v>
+      </c>
       <c r="D11" s="4">
         <f t="shared" si="0"/>
-        <v>4.5833333333333338E-4</v>
+        <v>7.0833333333333393E-5</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -632,12 +650,14 @@
     <row r="12" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="C12" s="4"/>
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.48299999999999998</v>
+      </c>
       <c r="D12" s="4">
         <f t="shared" si="0"/>
-        <v>5.0000000000000001E-4</v>
+        <v>9.9999999999999991E-5</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -652,12 +672,14 @@
     <row r="13" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="4">
-        <v>0.65</v>
-      </c>
-      <c r="C13" s="4"/>
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.495</v>
+      </c>
       <c r="D13" s="4">
         <f t="shared" si="0"/>
-        <v>5.4166666666666664E-4</v>
+        <v>1.3250000000000002E-4</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -672,12 +694,14 @@
     <row r="14" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="C14" s="4"/>
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.505</v>
+      </c>
       <c r="D14" s="4">
         <f t="shared" si="0"/>
-        <v>5.8333333333333327E-4</v>
+        <v>1.6583333333333329E-4</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -692,12 +716,14 @@
     <row r="15" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="C15" s="4"/>
+        <v>0.753</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.51300000000000001</v>
+      </c>
       <c r="D15" s="4">
         <f t="shared" si="0"/>
-        <v>6.2500000000000001E-4</v>
+        <v>1.9999999999999998E-4</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -712,12 +738,14 @@
     <row r="16" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="C16" s="4"/>
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.52</v>
+      </c>
       <c r="D16" s="4">
         <f t="shared" si="0"/>
-        <v>6.6666666666666675E-4</v>
+        <v>2.3583333333333336E-4</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -732,12 +760,14 @@
     <row r="17" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="C17" s="4"/>
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.53200000000000003</v>
+      </c>
       <c r="D17" s="4">
         <f t="shared" si="0"/>
-        <v>7.5000000000000002E-4</v>
+        <v>3.0833333333333331E-4</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -752,12 +782,14 @@
     <row r="18" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="4">
-        <v>1</v>
-      </c>
-      <c r="C18" s="4"/>
+        <v>1.002</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.54100000000000004</v>
+      </c>
       <c r="D18" s="4">
         <f t="shared" si="0"/>
-        <v>8.3333333333333339E-4</v>
+        <v>3.8416666666666666E-4</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -772,12 +804,14 @@
     <row r="19" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="C19" s="4"/>
+        <v>1.4990000000000001</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.57299999999999995</v>
+      </c>
       <c r="D19" s="4">
         <f t="shared" si="0"/>
-        <v>1.25E-3</v>
+        <v>7.7166666666666681E-4</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -792,12 +826,14 @@
     <row r="20" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="4">
-        <v>2</v>
-      </c>
-      <c r="C20" s="4"/>
+        <v>1.9950000000000001</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.59199999999999997</v>
+      </c>
       <c r="D20" s="4">
         <f t="shared" si="0"/>
-        <v>1.6666666666666668E-3</v>
+        <v>1.1691666666666667E-3</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>

</xml_diff>